<commit_message>
Fix/show patient details on forms (#221)
* fix: enrollment form validation

* feat: add patient details to forms
</commit_message>
<xml_diff>
--- a/itech-malawi/forms/app/patient_transferred.xlsx
+++ b/itech-malawi/forms/app/patient_transferred.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="85">
   <si>
     <t>type</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>../inputs/contact/phone</t>
+  </si>
+  <si>
+    <t>patient_phone</t>
+  </si>
+  <si>
+    <t>Patient Phone Number</t>
   </si>
   <si>
     <t>n</t>
@@ -161,6 +167,18 @@
   <si>
     <t xml:space="preserve">&lt;h4 style="color: #337ab7;"&gt;&lt;p&gt;Complete form if patient transferred clinic. Please note that the patient will no longer receive study messages when you submit this form.&lt;/p&gt;&lt;/h4&gt;
 </t>
+  </si>
+  <si>
+    <t>contact_name</t>
+  </si>
+  <si>
+    <t>&lt;h4&gt;Patient Name: ${patient_name}&lt;/h4&gt;</t>
+  </si>
+  <si>
+    <t>contact_phone</t>
+  </si>
+  <si>
+    <t>&lt;h4&gt;Patient Phone Number: ${patient_phone}&lt;/h4&gt;</t>
   </si>
   <si>
     <t>select_one yes_remindme_others</t>
@@ -1798,7 +1816,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Z18"/>
+  <dimension ref="A1:Z21"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2067,9 +2085,7 @@
         <v>32</v>
       </c>
       <c r="D7" s="13"/>
-      <c r="E7" t="s" s="14">
-        <v>20</v>
-      </c>
+      <c r="E7" s="14"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
@@ -2103,9 +2119,7 @@
         <v>34</v>
       </c>
       <c r="D8" s="13"/>
-      <c r="E8" t="s" s="14">
-        <v>20</v>
-      </c>
+      <c r="E8" s="14"/>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
@@ -2246,9 +2260,7 @@
       <c r="K12" t="s" s="30">
         <v>41</v>
       </c>
-      <c r="L12" t="s" s="30">
-        <v>20</v>
-      </c>
+      <c r="L12" s="30"/>
       <c r="M12" s="11"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
@@ -2301,26 +2313,26 @@
       <c r="Z13" s="32"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" t="s" s="33">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s" s="34">
+      <c r="A14" t="s" s="21">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s" s="22">
         <v>44</v>
       </c>
-      <c r="C14" t="s" s="35">
+      <c r="C14" t="s" s="23">
         <v>45</v>
       </c>
-      <c r="D14" s="36"/>
-      <c r="E14" t="s" s="34">
-        <v>16</v>
-      </c>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="37"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="24"/>
+      <c r="K14" t="s" s="23">
+        <v>43</v>
+      </c>
+      <c r="L14" s="25"/>
       <c r="M14" s="31"/>
       <c r="N14" s="32"/>
       <c r="O14" s="32"/>
@@ -2336,27 +2348,27 @@
       <c r="Y14" s="32"/>
       <c r="Z14" s="32"/>
     </row>
-    <row r="15" ht="228.75" customHeight="1">
+    <row r="15" ht="15.75" customHeight="1">
       <c r="A15" t="s" s="33">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s" s="34">
         <v>46</v>
       </c>
-      <c r="B15" t="s" s="34">
+      <c r="C15" t="s" s="35">
         <v>47</v>
       </c>
-      <c r="C15" t="s" s="38">
-        <v>48</v>
-      </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="40"/>
-      <c r="L15" t="s" s="41">
-        <v>20</v>
-      </c>
+      <c r="D15" s="36"/>
+      <c r="E15" t="s" s="34">
+        <v>16</v>
+      </c>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
       <c r="M15" s="31"/>
       <c r="N15" s="32"/>
       <c r="O15" s="32"/>
@@ -2372,27 +2384,27 @@
       <c r="Y15" s="32"/>
       <c r="Z15" s="32"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" ht="228.75" customHeight="1">
       <c r="A16" t="s" s="33">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s" s="34">
         <v>49</v>
       </c>
-      <c r="B16" t="s" s="34">
+      <c r="C16" t="s" s="38">
         <v>50</v>
-      </c>
-      <c r="C16" t="s" s="42">
-        <v>51</v>
       </c>
       <c r="D16" s="39"/>
       <c r="E16" s="39"/>
-      <c r="F16" t="s" s="42">
-        <v>30</v>
-      </c>
+      <c r="F16" s="39"/>
       <c r="G16" s="39"/>
       <c r="H16" s="39"/>
       <c r="I16" s="40"/>
       <c r="J16" s="39"/>
       <c r="K16" s="40"/>
-      <c r="L16" s="40"/>
+      <c r="L16" t="s" s="41">
+        <v>20</v>
+      </c>
       <c r="M16" s="31"/>
       <c r="N16" s="32"/>
       <c r="O16" s="32"/>
@@ -2410,21 +2422,17 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" t="s" s="33">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s" s="34">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s" s="42">
         <v>52</v>
       </c>
-      <c r="B17" t="s" s="34">
-        <v>53</v>
-      </c>
-      <c r="C17" t="s" s="43">
-        <v>54</v>
-      </c>
-      <c r="D17" t="s" s="42">
-        <v>55</v>
-      </c>
+      <c r="D17" s="39"/>
       <c r="E17" s="39"/>
-      <c r="F17" t="s" s="42">
-        <v>56</v>
-      </c>
+      <c r="F17" s="42"/>
       <c r="G17" s="39"/>
       <c r="H17" s="39"/>
       <c r="I17" s="40"/>
@@ -2447,21 +2455,25 @@
       <c r="Z17" s="32"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" t="s" s="44">
-        <v>35</v>
-      </c>
-      <c r="B18" s="45"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="46"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="47"/>
+      <c r="A18" t="s" s="33">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s" s="34">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s" s="42">
+        <v>54</v>
+      </c>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="31"/>
       <c r="N18" s="32"/>
       <c r="O18" s="32"/>
       <c r="P18" s="32"/>
@@ -2475,6 +2487,110 @@
       <c r="X18" s="32"/>
       <c r="Y18" s="32"/>
       <c r="Z18" s="32"/>
+    </row>
+    <row r="19" ht="15.75" customHeight="1">
+      <c r="A19" t="s" s="33">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s" s="34">
+        <v>56</v>
+      </c>
+      <c r="C19" t="s" s="42">
+        <v>57</v>
+      </c>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" t="s" s="42">
+        <v>30</v>
+      </c>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="31"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="32"/>
+      <c r="R19" s="32"/>
+      <c r="S19" s="32"/>
+      <c r="T19" s="32"/>
+      <c r="U19" s="32"/>
+      <c r="V19" s="32"/>
+      <c r="W19" s="32"/>
+      <c r="X19" s="32"/>
+      <c r="Y19" s="32"/>
+      <c r="Z19" s="32"/>
+    </row>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" t="s" s="33">
+        <v>58</v>
+      </c>
+      <c r="B20" t="s" s="34">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s" s="43">
+        <v>60</v>
+      </c>
+      <c r="D20" t="s" s="42">
+        <v>61</v>
+      </c>
+      <c r="E20" s="39"/>
+      <c r="F20" t="s" s="42">
+        <v>62</v>
+      </c>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="32"/>
+      <c r="Q20" s="32"/>
+      <c r="R20" s="32"/>
+      <c r="S20" s="32"/>
+      <c r="T20" s="32"/>
+      <c r="U20" s="32"/>
+      <c r="V20" s="32"/>
+      <c r="W20" s="32"/>
+      <c r="X20" s="32"/>
+      <c r="Y20" s="32"/>
+      <c r="Z20" s="32"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1">
+      <c r="A21" t="s" s="44">
+        <v>35</v>
+      </c>
+      <c r="B21" s="45"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="32"/>
+      <c r="Q21" s="32"/>
+      <c r="R21" s="32"/>
+      <c r="S21" s="32"/>
+      <c r="T21" s="32"/>
+      <c r="U21" s="32"/>
+      <c r="V21" s="32"/>
+      <c r="W21" s="32"/>
+      <c r="X21" s="32"/>
+      <c r="Y21" s="32"/>
+      <c r="Z21" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0" footer="0"/>
@@ -2502,7 +2618,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" t="s" s="49">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B1" t="s" s="49">
         <v>1</v>
@@ -2522,39 +2638,39 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" t="s" s="51">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s" s="51">
         <v>30</v>
       </c>
       <c r="C3" t="s" s="51">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" t="s" s="51">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s" s="51">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s" s="51">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" t="s" s="51">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s" s="52">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s" s="52">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -2622,31 +2738,31 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="57">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s" s="57">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C1" t="s" s="57">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D1" t="s" s="57">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E1" t="s" s="57">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="F1" t="s" s="57">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="G1" t="s" s="57">
         <v>1</v>
       </c>
       <c r="H1" t="s" s="57">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="I1" t="s" s="57">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="J1" s="57"/>
       <c r="K1" s="57"/>
@@ -2668,29 +2784,29 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" t="s" s="59">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s" s="60">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s" s="60">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s" s="60">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="E2" t="s" s="60">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="F2" s="61"/>
       <c r="G2" t="s" s="60">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="H2" t="s" s="60">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="I2" t="s" s="60">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="J2" s="61"/>
       <c r="K2" s="61"/>

</xml_diff>